<commit_message>
[ADD:양현지] use case description 추가
</commit_message>
<xml_diff>
--- a/usecase_diagram & usecase_description/use_case_description.xlsx
+++ b/usecase_diagram & usecase_description/use_case_description.xlsx
@@ -5,22 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93b1e4194ffc0e6e/바탕 화면/과제/소공/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\2023-1\소공\과제2\usecase_diagram &amp; usecase_description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{B7289B00-5B82-404B-AFF2-A2278A990A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E765A0DD-C16C-4461-B101-C1DCCB094A8B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461B11A0-D514-4435-9100-3D256B9B9A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="과제2-description" sheetId="2" r:id="rId1"/>
+    <sheet name="양현지_usecase_description" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="80">
   <si>
     <t>Actor Action</t>
   </si>
@@ -6230,12 +6231,801 @@
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>[지원 취소]</t>
+  </si>
+  <si>
+    <t>3. 취소 할 지원 정보를 선택</t>
+  </si>
+  <si>
+    <t>4. 취소 요청을 수행하며 취소 완료 메시지를 출력</t>
+  </si>
+  <si>
+    <t>[지원 정보 삭제]</t>
+  </si>
+  <si>
+    <t>3. 삭제 할 지원 정보를 선택</t>
+  </si>
+  <si>
+    <t>1. 회사 회원이 채용 정보 통계 요청</t>
+  </si>
+  <si>
+    <t>2. 일반 회원의 지원 정보(월별 지원횟수)를 마감시간 기준으로 출력</t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지원 횟수 정보 보기</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>등록한 모든</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>채용</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">정보에 대해 마감시간 기준으로 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>업무별</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지원자수</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>출력</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지원자수 정보 보기</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일반 회원이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지원횟수</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정보</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>요청</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일반 회원이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지원</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정보를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>조회</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일반</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">회원의 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지원 정보를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>회사이름</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>오름차순으로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>출력</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">일반 회원의 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지원정보를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>회사이름</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>오름차순으로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>출력</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>삭제</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>요청을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수행하며</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>삭제</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>완료</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>메시지를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>출력</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지원</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정보 선택</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일반 회원이 지원 정보를 선택</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지원 정보</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>조회</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -6349,6 +7139,51 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -6358,7 +7193,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -6428,11 +7263,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -6450,6 +7371,25 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -6465,10 +7405,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6674,23 +7610,23 @@
   </sheetPr>
   <dimension ref="A3:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="2" max="2" width="82.44140625" customWidth="1"/>
+    <col min="2" max="2" width="82.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="13">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="11"/>
     </row>
-    <row r="4" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="12.5">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -6698,37 +7634,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="12.5">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="12.5">
       <c r="A6" s="4"/>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="12.5">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="12.5">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="13">
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="11"/>
     </row>
-    <row r="10" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="12.5">
       <c r="A10" s="4" t="s">
         <v>0</v>
       </c>
@@ -6736,37 +7672,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="12.5">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="12.5">
       <c r="A12" s="4"/>
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="12.5">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="12.5">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="13">
       <c r="A15" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="11"/>
     </row>
-    <row r="16" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="12.5">
       <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
@@ -6774,25 +7710,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="12.5">
       <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="12.5">
       <c r="A18" s="4"/>
       <c r="B18" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="13">
       <c r="A19" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="11"/>
     </row>
-    <row r="20" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="12.5">
       <c r="A20" s="4" t="s">
         <v>0</v>
       </c>
@@ -6800,25 +7736,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="12.5">
       <c r="A21" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="12.5">
       <c r="A22" s="3"/>
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="13">
       <c r="A23" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="11"/>
     </row>
-    <row r="24" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="12.5">
       <c r="A24" s="4" t="s">
         <v>0</v>
       </c>
@@ -6826,29 +7762,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="12.5">
       <c r="A25" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="12.5">
       <c r="A26" s="3"/>
       <c r="B26" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="13">
       <c r="A28" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="11"/>
     </row>
-    <row r="29" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="12.5">
       <c r="A29" s="4" t="s">
         <v>0</v>
       </c>
@@ -6856,7 +7792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="12.5">
       <c r="A30" s="4" t="s">
         <v>23</v>
       </c>
@@ -6864,7 +7800,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="12.5">
       <c r="A31" s="4" t="s">
         <v>25</v>
       </c>
@@ -6872,19 +7808,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="12.5">
       <c r="A32" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="13">
       <c r="A33" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="11"/>
     </row>
-    <row r="34" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="12.5">
       <c r="A34" s="4" t="s">
         <v>0</v>
       </c>
@@ -6892,19 +7828,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="12.5">
       <c r="A35" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="13">
       <c r="A36" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="11"/>
     </row>
-    <row r="37" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="12.5">
       <c r="A37" s="4" t="s">
         <v>0</v>
       </c>
@@ -6912,7 +7848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="12.5">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -6920,7 +7856,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="12.5">
       <c r="A39" s="3" t="s">
         <v>32</v>
       </c>
@@ -6928,13 +7864,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" ht="16">
       <c r="A40" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B40" s="11"/>
     </row>
-    <row r="41" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="12.5">
       <c r="A41" s="4" t="s">
         <v>0</v>
       </c>
@@ -6942,7 +7878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="15.75" customHeight="1">
       <c r="A42" s="3" t="s">
         <v>34</v>
       </c>
@@ -6950,17 +7886,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="15.75" customHeight="1">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
     </row>
-    <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" ht="16">
       <c r="A44" s="12" t="s">
         <v>61</v>
       </c>
       <c r="B44" s="11"/>
     </row>
-    <row r="45" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="12.5">
       <c r="A45" s="4" t="s">
         <v>0</v>
       </c>
@@ -6968,7 +7904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="12.5">
       <c r="A46" s="6" t="s">
         <v>40</v>
       </c>
@@ -6976,13 +7912,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" ht="16">
       <c r="A47" s="12" t="s">
         <v>42</v>
       </c>
       <c r="B47" s="11"/>
     </row>
-    <row r="48" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="12.5">
       <c r="A48" s="4" t="s">
         <v>0</v>
       </c>
@@ -6990,7 +7926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" ht="16">
       <c r="A49" s="8" t="s">
         <v>43</v>
       </c>
@@ -6998,7 +7934,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="12.5">
       <c r="A50" s="6" t="s">
         <v>45</v>
       </c>
@@ -7006,13 +7942,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" ht="16">
       <c r="A51" s="12" t="s">
         <v>47</v>
       </c>
       <c r="B51" s="11"/>
     </row>
-    <row r="52" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="12.5">
       <c r="A52" s="4" t="s">
         <v>0</v>
       </c>
@@ -7020,7 +7956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="12.5">
       <c r="A53" s="8" t="s">
         <v>48</v>
       </c>
@@ -7028,7 +7964,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="12.5">
       <c r="A54" s="6" t="s">
         <v>50</v>
       </c>
@@ -7036,13 +7972,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="13">
       <c r="A55" s="12" t="s">
         <v>52</v>
       </c>
       <c r="B55" s="11"/>
     </row>
-    <row r="56" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="12.5">
       <c r="A56" s="4" t="s">
         <v>0</v>
       </c>
@@ -7050,7 +7986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="12.5">
       <c r="A57" s="6" t="s">
         <v>53</v>
       </c>
@@ -7058,13 +7994,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="13">
       <c r="A58" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B58" s="11"/>
     </row>
-    <row r="59" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="12.5">
       <c r="A59" s="4" t="s">
         <v>0</v>
       </c>
@@ -7072,7 +8008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="12.5">
       <c r="A60" s="6" t="s">
         <v>56</v>
       </c>
@@ -7080,13 +8016,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="13">
       <c r="A61" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B61" s="11"/>
     </row>
-    <row r="62" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="12.5">
       <c r="A62" s="4" t="s">
         <v>0</v>
       </c>
@@ -7094,7 +8030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="12.5">
       <c r="A63" s="3" t="s">
         <v>37</v>
       </c>
@@ -7102,13 +8038,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" ht="16">
       <c r="A64" s="12" t="s">
         <v>58</v>
       </c>
       <c r="B64" s="11"/>
     </row>
-    <row r="65" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="12.5">
       <c r="A65" s="4" t="s">
         <v>0</v>
       </c>
@@ -7116,7 +8052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="12.5">
       <c r="A66" s="6" t="s">
         <v>59</v>
       </c>
@@ -7126,6 +8062,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A23:B23"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A61:B61"/>
@@ -7137,13 +8078,281 @@
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A23:B23"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12814D97-8DD2-4A0D-8A61-4DB45C709AC5}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="65" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="48.90625" customWidth="1"/>
+    <col min="2" max="2" width="83.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="19" customHeight="1" thickBot="1">
+      <c r="A1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" ht="17" thickBot="1">
+      <c r="A2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="21" thickBot="1">
+      <c r="A3" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="17"/>
+    </row>
+    <row r="4" spans="1:4" ht="21" thickBot="1">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A5" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="18"/>
+    </row>
+    <row r="6" spans="1:4" ht="19" thickBot="1">
+      <c r="A6" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" spans="1:4" ht="17" thickBot="1">
+      <c r="A7" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="21" thickBot="1">
+      <c r="A8" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:4" ht="21" thickBot="1">
+      <c r="A9" s="18"/>
+      <c r="B9" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" thickBot="1">
+      <c r="A10" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="1:4" ht="17" thickBot="1">
+      <c r="A11" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" ht="21" thickBot="1">
+      <c r="A12" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" ht="33.5" customHeight="1" thickBot="1">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="1:4" ht="17" thickBot="1">
+      <c r="A14" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" spans="1:4" ht="17" thickBot="1">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+    </row>
+    <row r="16" spans="1:4" ht="17" thickBot="1">
+      <c r="A16" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="1:4" ht="17" thickBot="1">
+      <c r="A17" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="1:4" ht="21" thickBot="1">
+      <c r="A18" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="1:4" ht="21" thickBot="1">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:4" ht="17" thickBot="1">
+      <c r="A20" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+    </row>
+    <row r="21" spans="1:4" ht="21" thickBot="1">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:4" ht="19" customHeight="1" thickBot="1">
+      <c r="A22" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+    </row>
+    <row r="23" spans="1:4" ht="17" thickBot="1">
+      <c r="A23" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+    </row>
+    <row r="24" spans="1:4" ht="21" thickBot="1">
+      <c r="A24" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="17"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+    </row>
+    <row r="25" spans="1:4" ht="17" thickBot="1">
+      <c r="A25" s="18"/>
+      <c r="B25" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+    </row>
+    <row r="26" spans="1:4" ht="17" customHeight="1" thickBot="1">
+      <c r="A26" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+    </row>
+    <row r="27" spans="1:4" ht="17" thickBot="1">
+      <c r="A27" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+    </row>
+    <row r="28" spans="1:4" ht="17" thickBot="1">
+      <c r="A28" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+    </row>
+    <row r="29" spans="1:4" ht="21" thickBot="1">
+      <c r="A29" s="18"/>
+      <c r="B29" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+    </row>
+    <row r="30" spans="1:4" ht="16.5">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+    </row>
+    <row r="31" spans="1:4" ht="16.5">
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+    </row>
+    <row r="32" spans="1:4" ht="16.5">
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>